<commit_message>
Actualización asociación usuario entrevista
</commit_message>
<xml_diff>
--- a/src/main/resources/static/xls/plantilla_carga_basica.xlsx
+++ b/src/main/resources/static/xls/plantilla_carga_basica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usmcl-my.sharepoint.com/personal/jacob_vega_usm_cl/Documents/Proyectos/Entrevistas/Desarrollo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookair11/Documents/ProyectosSpringBoot/SA-entrevistas/entrevistas-sa/src/main/resources/static/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{0D3D0B18-63F8-E24E-A56C-29670A8F3790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EDC09DB-AC4C-3C41-BB37-277FB64E1A2E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86558BC-37B6-8940-ACEF-E13EDEB02B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Postulantes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Postulante ID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Fecha ingreso</t>
   </si>
   <si>
-    <t>Reclutador</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
@@ -70,15 +67,6 @@
     <t>CORREA</t>
   </si>
   <si>
-    <t>RECLUTADOR 1</t>
-  </si>
-  <si>
-    <t>RECLUTADOR 2</t>
-  </si>
-  <si>
-    <t>RECLUTADOR 3</t>
-  </si>
-  <si>
     <t>11.111.111-1</t>
   </si>
   <si>
@@ -158,6 +146,12 @@
   </si>
   <si>
     <t>BAEZA</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -244,9 +238,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -284,7 +278,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -390,7 +384,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -532,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,9 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -571,37 +563,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -611,38 +603,38 @@
       <c r="B2" s="2">
         <v>44562</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -652,38 +644,38 @@
       <c r="B3" s="2">
         <v>44594</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>17</v>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -693,38 +685,38 @@
       <c r="B4" s="2">
         <v>44623</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.25">

</xml_diff>